<commit_message>
Added new offset system: FactorOffsetOptions
</commit_message>
<xml_diff>
--- a/Assets/Resources/visualisation_combinaison.xlsx
+++ b/Assets/Resources/visualisation_combinaison.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D96513-AE55-450B-90A4-399E2FFDAFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E5D237-4F9F-4833-910C-F3707389023D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XLSX" sheetId="1" r:id="rId1"/>
     <sheet name="CSVforUnity" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1062,6 +1075,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1076,15 +1098,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3751,26 +3764,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="80" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="78"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="75" t="s">
+      <c r="L1" s="81"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="75"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="77" t="s">
+      <c r="O1" s="78"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="78"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="77" t="s">
+      <c r="R1" s="81"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="78"/>
-      <c r="V1" s="79"/>
+      <c r="U1" s="81"/>
+      <c r="V1" s="82"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
@@ -4289,11 +4302,11 @@
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="79"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="82"/>
     </row>
     <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="33" t="s">
@@ -4397,7 +4410,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="80" t="str">
+      <c r="A24" s="75" t="str">
         <f>A3</f>
         <v>point R</v>
       </c>
@@ -4418,7 +4431,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="81"/>
+      <c r="A25" s="76"/>
       <c r="B25" s="69" t="s">
         <v>43</v>
       </c>
@@ -4436,7 +4449,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="82"/>
+      <c r="A26" s="77"/>
       <c r="B26" s="70" t="s">
         <v>44</v>
       </c>
@@ -4454,7 +4467,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="80" t="str">
+      <c r="A27" s="75" t="str">
         <f>A4</f>
         <v>point ++</v>
       </c>
@@ -4475,7 +4488,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="81"/>
+      <c r="A28" s="76"/>
       <c r="B28" s="69" t="s">
         <v>43</v>
       </c>
@@ -4493,7 +4506,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="82"/>
+      <c r="A29" s="77"/>
       <c r="B29" s="70" t="s">
         <v>44</v>
       </c>
@@ -4511,7 +4524,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="80" t="str">
+      <c r="A30" s="75" t="str">
         <f>A5</f>
         <v>point --</v>
       </c>
@@ -4532,7 +4545,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="81"/>
+      <c r="A31" s="76"/>
       <c r="B31" s="69" t="s">
         <v>43</v>
       </c>
@@ -4550,7 +4563,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="82"/>
+      <c r="A32" s="77"/>
       <c r="B32" s="70" t="s">
         <v>44</v>
       </c>
@@ -4568,7 +4581,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="80" t="str">
+      <c r="A33" s="75" t="str">
         <f>A6</f>
         <v>point +-</v>
       </c>
@@ -4589,7 +4602,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="81"/>
+      <c r="A34" s="76"/>
       <c r="B34" s="69" t="s">
         <v>43</v>
       </c>
@@ -4607,7 +4620,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="82"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="70" t="s">
         <v>44</v>
       </c>
@@ -4625,7 +4638,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="80" t="str">
+      <c r="A36" s="75" t="str">
         <f>A7</f>
         <v>point -+</v>
       </c>
@@ -4646,7 +4659,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="81"/>
+      <c r="A37" s="76"/>
       <c r="B37" s="69" t="s">
         <v>43</v>
       </c>
@@ -4664,7 +4677,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="82"/>
+      <c r="A38" s="77"/>
       <c r="B38" s="70" t="s">
         <v>44</v>
       </c>
@@ -4696,16 +4709,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="B14:D14"/>
     <mergeCell ref="A24:A26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>